<commit_message>
20220621 - pins configuration changed.
</commit_message>
<xml_diff>
--- a/Documents/glcd_pin_configuration.xlsx
+++ b/Documents/glcd_pin_configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehdi\GitHub\EDVDU\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehdi\Documents\GitHub\EDVDU\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>GLCD_D0</t>
   </si>
@@ -182,25 +182,22 @@
     <t>GLCD_PSB</t>
   </si>
   <si>
-    <t>SPI_NSS</t>
-  </si>
-  <si>
-    <t>SPI_MOSI</t>
-  </si>
-  <si>
-    <t>SPI_SCK</t>
-  </si>
-  <si>
     <t>PB8</t>
   </si>
   <si>
     <t>PB9</t>
   </si>
   <si>
-    <t>NRST</t>
-  </si>
-  <si>
     <t>RESET</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>PB15</t>
+  </si>
+  <si>
+    <t>PB13</t>
   </si>
 </sst>
 </file>
@@ -812,7 +809,7 @@
   <dimension ref="B1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +898,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G7" s="2">
         <v>17</v>
@@ -921,7 +918,7 @@
         <v>48</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G8" s="2">
         <v>16</v>
@@ -941,7 +938,7 @@
         <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2">
         <v>18</v>
@@ -1105,7 +1102,7 @@
         <v>51</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2">
         <v>14</v>
@@ -1123,7 +1120,7 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G19" s="2">
         <v>15</v>
@@ -1143,10 +1140,10 @@
         <v>13</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>